<commit_message>
some of my most-used ones :)
</commit_message>
<xml_diff>
--- a/MiscVBAFunctions/MiscVBAFunctions.xlsx
+++ b/MiscVBAFunctions/MiscVBAFunctions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\AppData\Local\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malan\AppData\Local\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C55A3DCD-6BF0-4FD7-968A-DFAE62A03FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0CCD4BB-29B8-40F2-92CD-27D6334297D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3750" yWindow="1545" windowWidth="20040" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -341,10 +341,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add grouping functionality based on indentation lvls
</commit_message>
<xml_diff>
--- a/MiscVBAFunctions/MiscVBAFunctions.xlsx
+++ b/MiscVBAFunctions/MiscVBAFunctions.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malan\AppData\Local\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B56E674-51CA-4550-93DB-943F79125522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8B32AD8-C896-4CEA-8A08-3FD00A20EB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1644" yWindow="1644" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="648" yWindow="696" windowWidth="21600" windowHeight="11400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TableToDicts" sheetId="1" r:id="rId1"/>
+    <sheet name="GroupOnIndentations" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="__TestGroupColumnsOnIndentations__">GroupOnIndentations!$D$5:$G$5</definedName>
+    <definedName name="__TestGroupRowsOnIndentations__">GroupOnIndentations!$C$6:$C$12</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>a</t>
   </si>
@@ -46,6 +51,30 @@
   </si>
   <si>
     <t>TableToDictsTestData</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>zz</t>
   </si>
 </sst>
 </file>
@@ -81,8 +110,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,8 +413,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -428,4 +463,72 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E7B102-832D-491A-8D40-8A408C7C8322}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="C5:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="6" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C7" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C11" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added general collection functions
Added min() max() mean() functions for collections.
</commit_message>
<xml_diff>
--- a/MiscVBAFunctions/MiscVBAFunctions.xlsx
+++ b/MiscVBAFunctions/MiscVBAFunctions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malan\AppData\Local\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uni\AppData\Local\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8B32AD8-C896-4CEA-8A08-3FD00A20EB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6E102DC-6FC9-42DF-8B1B-13A93EE0E89A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="648" yWindow="696" windowWidth="21600" windowHeight="11400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3555" yWindow="2100" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TableToDicts" sheetId="1" r:id="rId1"/>
@@ -417,14 +417,14 @@
       <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -435,7 +435,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1</v>
       </c>
@@ -446,7 +446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>4</v>
       </c>
@@ -471,15 +471,15 @@
   <dimension ref="C5:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="6" width="8.88671875" customWidth="1"/>
+    <col min="5" max="6" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>8</v>
       </c>
@@ -493,37 +493,37 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
revert to master .xlsx binary
</commit_message>
<xml_diff>
--- a/MiscVBAFunctions/MiscVBAFunctions.xlsx
+++ b/MiscVBAFunctions/MiscVBAFunctions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uni\AppData\Local\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malan\AppData\Local\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70BDBA19-C0C3-4612-B7FA-43B5FB42981B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8B32AD8-C896-4CEA-8A08-3FD00A20EB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="2100" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="648" yWindow="696" windowWidth="21600" windowHeight="11400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TableToDicts" sheetId="1" r:id="rId1"/>
@@ -417,14 +417,14 @@
       <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -435,7 +435,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>1</v>
       </c>
@@ -446,7 +446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>4</v>
       </c>
@@ -474,12 +474,12 @@
       <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="6" width="8.85546875" customWidth="1"/>
+    <col min="5" max="6" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>8</v>
       </c>
@@ -493,37 +493,37 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Added value to test_zip() test
</commit_message>
<xml_diff>
--- a/MiscVBAFunctions/MiscVBAFunctions.xlsx
+++ b/MiscVBAFunctions/MiscVBAFunctions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uni\AppData\Local\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC747E7F-191C-468B-9585-126A736E6067}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{81C57B8E-6247-4A4E-8392-AF855BAE624F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="1020" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -471,7 +471,7 @@
   <dimension ref="C5:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Replaced Sheets with Worksheets
</commit_message>
<xml_diff>
--- a/MiscVBAFunctions/MiscVBAFunctions.xlsx
+++ b/MiscVBAFunctions/MiscVBAFunctions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uni\AppData\Local\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88357981-C491-4DDF-8FA7-77FCE4CD8F4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9B3C5E8-C62E-40BA-A98F-5344A2F3A5DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="1020" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2670" yWindow="2115" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TableToDicts" sheetId="1" r:id="rId1"/>
@@ -471,7 +471,7 @@
   <dimension ref="C5:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Unit tests for EnsureDictI
</commit_message>
<xml_diff>
--- a/MiscVBAFunctions/MiscVBAFunctions.xlsx
+++ b/MiscVBAFunctions/MiscVBAFunctions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uni\AppData\Local\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9B3C5E8-C62E-40BA-A98F-5344A2F3A5DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{53875199-7060-41E8-8853-EFEE68347334}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2670" yWindow="2115" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -471,7 +471,7 @@
   <dimension ref="C5:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
moved tabletodicts to testing book
</commit_message>
<xml_diff>
--- a/MiscVBAFunctions/MiscVBAFunctions.xlsx
+++ b/MiscVBAFunctions/MiscVBAFunctions.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uni\AppData\Local\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malan\AppData\Local\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5162277E-1BD7-493F-A40F-076E8B6F3192}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{67747748-71A6-40A4-8ED3-E920CAD18ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3105" yWindow="-12720" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="624" yWindow="0" windowWidth="20448" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TableToDicts" sheetId="1" r:id="rId1"/>
-    <sheet name="GroupOnIndentations" sheetId="2" r:id="rId2"/>
+    <sheet name="GroupOnIndentations" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="__TestGroupColumnsOnIndentations__">GroupOnIndentations!$D$5:$G$5</definedName>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>a</t>
   </si>
@@ -48,9 +47,6 @@
   </si>
   <si>
     <t>c</t>
-  </si>
-  <si>
-    <t>TableToDictsTestData</t>
   </si>
   <si>
     <t>d</t>
@@ -133,18 +129,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C5FDB0C3-06FA-485B-A438-72E9C8081166}" name="TableToDictsTestData" displayName="TableToDictsTestData" ref="B4:D6" totalsRowShown="0">
-  <autoFilter ref="B4:D6" xr:uid="{C5FDB0C3-06FA-485B-A438-72E9C8081166}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{C21F091C-0125-4667-B78C-241039B31DF4}" name="a"/>
-    <tableColumn id="2" xr3:uid="{1EFBE33F-EDB5-4D25-8068-17F74FE6562D}" name="b"/>
-    <tableColumn id="3" xr3:uid="{477DA29F-B7BF-4C42-8F77-2A1EC51E5F06}" name="c"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -409,124 +393,67 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E7B102-832D-491A-8D40-8A408C7C8322}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="C5:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="8.85546875" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="8.85546875" customWidth="1" outlineLevel="2"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="8.88671875" customWidth="1" outlineLevel="2"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" t="s">
         <v>10</v>
       </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="3:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:7" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:7" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="3:7" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
+    <row r="11" spans="3:7" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="3:7" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="C11" s="2" t="s">
+    <row r="12" spans="3:7" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="C12" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="3:7" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="C12" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move group on indentations to another workbook
</commit_message>
<xml_diff>
--- a/MiscVBAFunctions/MiscVBAFunctions.xlsx
+++ b/MiscVBAFunctions/MiscVBAFunctions.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malan\AppData\Local\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67747748-71A6-40A4-8ED3-E920CAD18ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C19C5E21-E1DA-416A-8C7D-09C9668320D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="624" yWindow="0" windowWidth="20448" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="GroupOnIndentations" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <definedNames>
-    <definedName name="__TestGroupColumnsOnIndentations__">GroupOnIndentations!$D$5:$G$5</definedName>
-    <definedName name="__TestGroupRowsOnIndentations__">GroupOnIndentations!$C$6:$C$12</definedName>
+    <definedName name="__TestGroupColumnsOnIndentations__">[1]GroupOnIndentations!$D$5:$G$5</definedName>
+    <definedName name="__TestGroupRowsOnIndentations__">[1]GroupOnIndentations!$C$6:$C$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,44 +38,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>z</t>
-  </si>
-  <si>
-    <t>zz</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -106,14 +71,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -129,6 +88,69 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="GroupOnIndentations"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="5">
+          <cell r="D5" t="str">
+            <v>x</v>
+          </cell>
+          <cell r="E5" t="str">
+            <v>y</v>
+          </cell>
+          <cell r="F5" t="str">
+            <v>z</v>
+          </cell>
+          <cell r="G5" t="str">
+            <v>zz</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="C6" t="str">
+            <v>a</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7" t="str">
+            <v>b</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="C8" t="str">
+            <v>c</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="C9" t="str">
+            <v>d</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="C10" t="str">
+            <v>e</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11" t="str">
+            <v>f</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12" t="str">
+            <v>g</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -393,70 +415,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E7B102-832D-491A-8D40-8A408C7C8322}">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="C5:G12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4ADDDA4-6550-4D51-B958-0ED7B874B8B7}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="2" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" width="8.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="8.88671875" customWidth="1" outlineLevel="2"/>
-  </cols>
-  <sheetData>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="3:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="3:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="3:7" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="C11" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="3:7" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="C12" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove unused named ranges from Excel file
</commit_message>
<xml_diff>
--- a/MiscVBAFunctions/MiscVBAFunctions.xlsx
+++ b/MiscVBAFunctions/MiscVBAFunctions.xlsx
@@ -8,20 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malan\AppData\Local\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C19C5E21-E1DA-416A-8C7D-09C9668320D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E95AAC6C-727D-4E7A-9825-9B4F64980B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="624" yWindow="0" windowWidth="20448" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1428" yWindow="1428" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
-  <definedNames>
-    <definedName name="__TestGroupColumnsOnIndentations__">[1]GroupOnIndentations!$D$5:$G$5</definedName>
-    <definedName name="__TestGroupRowsOnIndentations__">[1]GroupOnIndentations!$C$6:$C$12</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -88,69 +81,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="GroupOnIndentations"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="5">
-          <cell r="D5" t="str">
-            <v>x</v>
-          </cell>
-          <cell r="E5" t="str">
-            <v>y</v>
-          </cell>
-          <cell r="F5" t="str">
-            <v>z</v>
-          </cell>
-          <cell r="G5" t="str">
-            <v>zz</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="C6" t="str">
-            <v>a</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7" t="str">
-            <v>b</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="C8" t="str">
-            <v>c</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="C9" t="str">
-            <v>d</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="C10" t="str">
-            <v>e</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11" t="str">
-            <v>f</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12" t="str">
-            <v>g</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -419,7 +349,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>

<commit_message>
remove `foo` named range
</commit_message>
<xml_diff>
--- a/MiscVBAFunctions/MiscVBAFunctions.xlsx
+++ b/MiscVBAFunctions/MiscVBAFunctions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malan\AppData\Local\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E95AAC6C-727D-4E7A-9825-9B4F64980B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{248DC2C7-1EFF-4277-921D-7AF7BA012A57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1428" yWindow="1428" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -350,7 +350,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added UnitTests for all modules.
</commit_message>
<xml_diff>
--- a/MiscVBAFunctions/MiscVBAFunctions.xlsx
+++ b/MiscVBAFunctions/MiscVBAFunctions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uni\AppData\Local\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69DB2B56-F542-40B3-9001-BCA4C9C76BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BB26F7F-D386-4D2A-B837-835BF0CE7B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30135" yWindow="2595" windowWidth="24585" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="645" yWindow="1695" windowWidth="24585" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -350,7 +350,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated module to convert Range to 2D array
</commit_message>
<xml_diff>
--- a/MiscVBAFunctions/MiscVBAFunctions.xlsx
+++ b/MiscVBAFunctions/MiscVBAFunctions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uni\AppData\Local\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BB26F7F-D386-4D2A-B837-835BF0CE7B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B61E5CCB-C821-44F0-AA10-05CBF9D7D662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="645" yWindow="1695" windowWidth="24585" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33015" yWindow="0" windowWidth="24585" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -350,7 +350,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changed printAllEarlyBindings to a private sub.
</commit_message>
<xml_diff>
--- a/MiscVBAFunctions/MiscVBAFunctions.xlsx
+++ b/MiscVBAFunctions/MiscVBAFunctions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uni\AppData\Local\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B61E5CCB-C821-44F0-AA10-05CBF9D7D662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{362FBE9A-AE3B-4DA3-92CF-850AC93C6C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33015" yWindow="0" windowWidth="24585" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -350,7 +350,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added Path() function in the newly created MiscOs module.
</commit_message>
<xml_diff>
--- a/MiscVBAFunctions/MiscVBAFunctions.xlsx
+++ b/MiscVBAFunctions/MiscVBAFunctions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uni\AppData\Local\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{362FBE9A-AE3B-4DA3-92CF-850AC93C6C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBB29E24-AD9A-45CC-90C4-10E50B356386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33015" yWindow="0" windowWidth="24585" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33015" yWindow="1035" windowWidth="24585" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -350,7 +350,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
revert to binary on main branch
</commit_message>
<xml_diff>
--- a/MiscVBAFunctions/MiscVBAFunctions.xlsx
+++ b/MiscVBAFunctions/MiscVBAFunctions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uni\AppData\Local\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBB29E24-AD9A-45CC-90C4-10E50B356386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{362FBE9A-AE3B-4DA3-92CF-850AC93C6C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33015" yWindow="1035" windowWidth="24585" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33015" yWindow="0" windowWidth="24585" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -350,7 +350,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added extra OS functions. Unit tests not yet added.
</commit_message>
<xml_diff>
--- a/MiscVBAFunctions/MiscVBAFunctions.xlsx
+++ b/MiscVBAFunctions/MiscVBAFunctions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uni\AppData\Local\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{362FBE9A-AE3B-4DA3-92CF-850AC93C6C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9432CCC3-700C-48AA-8966-0D06753002D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33015" yWindow="0" windowWidth="24585" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35865" yWindow="1035" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -350,7 +350,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Glob and RGlob functional
</commit_message>
<xml_diff>
--- a/MiscVBAFunctions/MiscVBAFunctions.xlsx
+++ b/MiscVBAFunctions/MiscVBAFunctions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uni\AppData\Local\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F905423B-EFEB-4343-872D-C23FD2DF1426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B082E02B-066C-42E4-96B8-3F61BBDB8206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1230" yWindow="3345" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>

</xml_diff>

<commit_message>
Add IgnoreCaseValues option to GetTableRowIndex
</commit_message>
<xml_diff>
--- a/MiscVBAFunctions/MiscVBAFunctions.xlsx
+++ b/MiscVBAFunctions/MiscVBAFunctions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uni\AppData\Local\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\AppData\Local\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B082E02B-066C-42E4-96B8-3F61BBDB8206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9EF84BFA-6103-44E4-AC4F-5A844F8EE039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="3345" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2220" yWindow="345" windowWidth="31005" windowHeight="14010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>

</xml_diff>

<commit_message>
Bugfix case sensitive inverse
</commit_message>
<xml_diff>
--- a/MiscVBAFunctions/MiscVBAFunctions.xlsx
+++ b/MiscVBAFunctions/MiscVBAFunctions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\AppData\Local\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ABF8D3B0-3BFA-4310-84D6-C470407607A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{11AF33C7-8107-4523-8048-31B5535205EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="345" windowWidth="31005" windowHeight="14010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -350,7 +350,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>